<commit_message>
Bought 5 pieces of MPU6500
</commit_message>
<xml_diff>
--- a/Finance/PROJ324 Expenditure Breakdown.xlsx
+++ b/Finance/PROJ324 Expenditure Breakdown.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE2AFAA-B913-439A-9ECF-B014D55C5186}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC64CAC-4FAA-4B1F-BA59-C313A0590969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>5pcs GY-6500 MPU6500</t>
+  </si>
+  <si>
+    <t>Banggood</t>
+  </si>
+  <si>
+    <t>Click Here</t>
   </si>
 </sst>
 </file>
@@ -105,9 +114,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -389,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,18 +469,139 @@
       </c>
       <c r="H2">
         <f>SUM(D2:D50)</f>
-        <v>9.98</v>
+        <v>21.09</v>
       </c>
       <c r="I2">
         <f>SUM(300-H2)</f>
-        <v>290.02</v>
+        <v>278.91000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>11.11</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D19" si="0">SUM(C3*B3)</f>
+        <v>11.11</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43514</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{49777C7F-45EE-4562-A32E-F2B70F13CE0D}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{8C172490-B37A-4063-A563-3B2DDBA9E667}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Purchased TB6600 stepper drivers and 24V 20A power supply
</commit_message>
<xml_diff>
--- a/Finance/PROJ324 Expenditure Breakdown.xlsx
+++ b/Finance/PROJ324 Expenditure Breakdown.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3FC205-11D7-4521-AAB1-508F8019DF85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043A7733-9AB6-4449-8FE8-3E4E76A72C94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Switching Power Supply 24V 20A</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>3PCS TB6600 4A 9-42V Stepper Motor Driver</t>
   </si>
 </sst>
 </file>
@@ -408,12 +417,12 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
@@ -475,11 +484,11 @@
       </c>
       <c r="H2">
         <f>SUM(D2:D50)</f>
-        <v>71.08</v>
+        <v>132.06</v>
       </c>
       <c r="I2">
         <f>SUM(300-H2)</f>
-        <v>228.92000000000002</v>
+        <v>167.94</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -531,15 +540,51 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>37.99</v>
+      </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37.99</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43532</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>22.99</v>
+      </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.99</v>
+      </c>
+      <c r="E6" s="2">
+        <v>43532</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -625,8 +670,10 @@
     <hyperlink ref="G2" r:id="rId1" xr:uid="{49777C7F-45EE-4562-A32E-F2B70F13CE0D}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{8C172490-B37A-4063-A563-3B2DDBA9E667}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{97D69B75-1040-44FD-ABA7-F0DCB8FA0E83}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{B9570FCE-ABDE-41AE-A336-B999E3E198BE}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{B22EDB9C-2F75-4AA0-85A4-44C576D55407}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-adding the latest expenditure breakdown as last one was accidentally deleted
</commit_message>
<xml_diff>
--- a/Finance/PROJ324 Expenditure Breakdown.xlsx
+++ b/Finance/PROJ324 Expenditure Breakdown.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043A7733-9AB6-4449-8FE8-3E4E76A72C94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11214070-2110-47F8-9A83-2AD26E0083B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://uk.rs-online.com/web/p/processor-microcontroller-development-kits/1438574/</t>
-  </si>
-  <si>
     <t>RS Online</t>
   </si>
   <si>
@@ -85,6 +82,30 @@
   </si>
   <si>
     <t>3PCS TB6600 4A 9-42V Stepper Motor Driver</t>
+  </si>
+  <si>
+    <t>5mm Bore Braid Sleeving x 500mm</t>
+  </si>
+  <si>
+    <t>100 Pack of Black Cable Ties - 200mm x 2.5mm</t>
+  </si>
+  <si>
+    <t>2pcs 1s 3.7V 650mAh Lipo Battery with USB Charger</t>
+  </si>
+  <si>
+    <t>HiLetgo CP2102 USB 2.0 to TTL 5PIN Serial Converter</t>
+  </si>
+  <si>
+    <t>Kamtop Dupont Crimping Tools </t>
+  </si>
+  <si>
+    <t>Hook and Loop Reusable Fastening Cable</t>
+  </si>
+  <si>
+    <t>5x WHITE Mini 170 Tie Point Solderless Breadboard</t>
+  </si>
+  <si>
+    <t>ZY-55 7 Breadboard Set</t>
   </si>
 </sst>
 </file>
@@ -417,12 +438,12 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
@@ -456,7 +477,7 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -477,23 +498,23 @@
         <v>9.98</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <f>SUM(D2:D50)</f>
-        <v>132.06</v>
+        <v>191.48000000000005</v>
       </c>
       <c r="I2">
         <f>SUM(300-H2)</f>
-        <v>167.94</v>
+        <v>108.51999999999995</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -509,15 +530,15 @@
         <v>43514</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -533,15 +554,15 @@
         <v>43526</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -557,15 +578,15 @@
         <v>43532</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -581,58 +602,202 @@
         <v>43532</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2.99</v>
+      </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.99</v>
+      </c>
+      <c r="E7" s="2">
+        <v>43549</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3.89</v>
+      </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.89</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43549</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>22.99</v>
+      </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C9*B9)</f>
+        <v>22.99</v>
+      </c>
+      <c r="E9" s="2">
+        <v>43550</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>9.99</v>
+      </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C10*B10)</f>
+        <v>9.99</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43550</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1.81</v>
+      </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C11*B11)</f>
+        <v>5.43</v>
+      </c>
+      <c r="E11" s="2">
+        <v>43557</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2.99</v>
+      </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C12*B12)</f>
+        <v>2.99</v>
+      </c>
+      <c r="E12" s="2">
+        <v>43557</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>7.99</v>
+      </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C13*B13)</f>
+        <v>7.99</v>
+      </c>
+      <c r="E13" s="2">
+        <v>43559</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>3.15</v>
+      </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C14*B14)</f>
+        <v>3.15</v>
+      </c>
+      <c r="E14" s="2">
+        <v>43561</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,13 +832,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{49777C7F-45EE-4562-A32E-F2B70F13CE0D}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{8C172490-B37A-4063-A563-3B2DDBA9E667}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{97D69B75-1040-44FD-ABA7-F0DCB8FA0E83}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{B9570FCE-ABDE-41AE-A336-B999E3E198BE}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{B22EDB9C-2F75-4AA0-85A4-44C576D55407}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{8C172490-B37A-4063-A563-3B2DDBA9E667}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{97D69B75-1040-44FD-ABA7-F0DCB8FA0E83}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{B9570FCE-ABDE-41AE-A336-B999E3E198BE}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{B22EDB9C-2F75-4AA0-85A4-44C576D55407}"/>
+    <hyperlink ref="G11" r:id="rId5" xr:uid="{6464F753-3745-4B70-ABE8-4ACBE9D4BD58}"/>
+    <hyperlink ref="G12" r:id="rId6" xr:uid="{17DFA971-19E9-44B2-8EE8-6F58E8BB1893}"/>
+    <hyperlink ref="G13" r:id="rId7" xr:uid="{78EE4D1E-32FD-4F57-A481-CE20CB19BA42}"/>
+    <hyperlink ref="G14" r:id="rId8" xr:uid="{6C1CED2F-CF62-4DAD-8C20-35433991F4F9}"/>
+    <hyperlink ref="G9" r:id="rId9" xr:uid="{A1BEDF37-2264-4763-A474-750646B50E1F}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{6F8472DC-94EA-4F26-AB1A-528D537DA910}"/>
+    <hyperlink ref="G7" r:id="rId11" xr:uid="{1758DA28-ACD7-4871-A229-CDEE2D18F2C4}"/>
+    <hyperlink ref="G8" r:id="rId12" xr:uid="{64A6A024-7F67-4FE8-900B-5938C27A0B98}"/>
+    <hyperlink ref="G2" r:id="rId13" xr:uid="{9325C0F9-B74D-4FFA-B5C8-18A4598B5322}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the finance table
</commit_message>
<xml_diff>
--- a/Finance/PROJ324 Expenditure Breakdown.xlsx
+++ b/Finance/PROJ324 Expenditure Breakdown.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11214070-2110-47F8-9A83-2AD26E0083B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474E93AE-2CE7-4391-BB88-80A21676EE69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>ZY-55 7 Breadboard Set</t>
+  </si>
+  <si>
+    <t>Right angle mini usb cable</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,11 +508,11 @@
       </c>
       <c r="H2">
         <f>SUM(D2:D50)</f>
-        <v>191.48000000000005</v>
+        <v>193.87000000000003</v>
       </c>
       <c r="I2">
         <f>SUM(300-H2)</f>
-        <v>108.51999999999995</v>
+        <v>106.12999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,7 +670,7 @@
         <v>22.99</v>
       </c>
       <c r="D9">
-        <f>SUM(C9*B9)</f>
+        <f t="shared" ref="D9:D14" si="1">SUM(C9*B9)</f>
         <v>22.99</v>
       </c>
       <c r="E9" s="2">
@@ -691,7 +694,7 @@
         <v>9.99</v>
       </c>
       <c r="D10">
-        <f>SUM(C10*B10)</f>
+        <f t="shared" si="1"/>
         <v>9.99</v>
       </c>
       <c r="E10" s="2">
@@ -715,7 +718,7 @@
         <v>1.81</v>
       </c>
       <c r="D11">
-        <f>SUM(C11*B11)</f>
+        <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
       <c r="E11" s="2">
@@ -739,7 +742,7 @@
         <v>2.99</v>
       </c>
       <c r="D12">
-        <f>SUM(C12*B12)</f>
+        <f t="shared" si="1"/>
         <v>2.99</v>
       </c>
       <c r="E12" s="2">
@@ -763,7 +766,7 @@
         <v>7.99</v>
       </c>
       <c r="D13">
-        <f>SUM(C13*B13)</f>
+        <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
       <c r="E13" s="2">
@@ -787,7 +790,7 @@
         <v>3.15</v>
       </c>
       <c r="D14">
-        <f>SUM(C14*B14)</f>
+        <f t="shared" si="1"/>
         <v>3.15</v>
       </c>
       <c r="E14" s="2">
@@ -801,9 +804,27 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2.39</v>
+      </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.39</v>
+      </c>
+      <c r="E15" s="2">
+        <v>43583</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -845,8 +866,9 @@
     <hyperlink ref="G7" r:id="rId11" xr:uid="{1758DA28-ACD7-4871-A229-CDEE2D18F2C4}"/>
     <hyperlink ref="G8" r:id="rId12" xr:uid="{64A6A024-7F67-4FE8-900B-5938C27A0B98}"/>
     <hyperlink ref="G2" r:id="rId13" xr:uid="{9325C0F9-B74D-4FFA-B5C8-18A4598B5322}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{BE1B61C2-FFEE-46D2-B86F-298E1AE38C52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>